<commit_message>
RBA v1.2 - Arquivo gerar_novo_modelo_convocacao Atualizado
</commit_message>
<xml_diff>
--- a/ArquivosGerados/dados_filtrados_com_RA_e_Nome_e_Série.xlsx
+++ b/ArquivosGerados/dados_filtrados_com_RA_e_Nome_e_Série.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,6 +1029,110 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cauan De Oliveira Campos</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>13</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>44960</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="K12" t="n">
+        <v>31026932</v>
+      </c>
+      <c r="L12" t="n">
+        <v>900086943667</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>000113555719 - 6</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>8° ANO B INTEGRAL ANUAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>39</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ian Lucas Alves Silva Moura</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>14</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="K13" t="n">
+        <v>30092959</v>
+      </c>
+      <c r="L13" t="n">
+        <v>900108744400</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>000112621744 - X</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>8° ANO B INTEGRAL ANUAL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>